<commit_message>
Checking if suggest currency form works
</commit_message>
<xml_diff>
--- a/cypress/downloads/relatorio-cotacoes.xlsx
+++ b/cypress/downloads/relatorio-cotacoes.xlsx
@@ -157,10 +157,10 @@
     <t xml:space="preserve">Horário do relatório</t>
   </si>
   <si>
-    <t xml:space="preserve">17/04/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04:34</t>
+    <t xml:space="preserve">18/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03:18</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>5.29</v>
+        <v>5.23</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>5</v>
@@ -629,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>3.37</v>
+        <v>3.39</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>8</v>
@@ -643,7 +643,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>3.81</v>
+        <v>3.83</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>10</v>
@@ -657,7 +657,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>5.59</v>
+        <v>5.62</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>12</v>
@@ -671,7 +671,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>5.77</v>
+        <v>5.79</v>
       </c>
       <c r="C6" t="s" s="2">
         <v>15</v>
@@ -685,7 +685,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="3">
-        <v>0.0342</v>
+        <v>0.0339</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>18</v>
@@ -699,7 +699,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="3">
-        <v>6.57</v>
+        <v>6.52</v>
       </c>
       <c r="C8" t="s" s="2">
         <v>21</v>
@@ -713,7 +713,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3">
-        <v>1.41</v>
+        <v>1.39</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>24</v>
@@ -797,7 +797,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="3">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>38</v>

</xml_diff>